<commit_message>
Added 4.5 and 4.6. Results completed, but still need to do more tables and a few more figures.
</commit_message>
<xml_diff>
--- a/assets_output/4.5_returns.xlsx
+++ b/assets_output/4.5_returns.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
   <si>
     <t>Table 4.3: Returns at periods of time after routes ended (per route)</t>
   </si>
@@ -47,6 +47,51 @@
   </si>
   <si>
     <t>% not returned</t>
+  </si>
+  <si>
+    <t>Table A.8: Returns at periods of time after exit by end reason</t>
+  </si>
+  <si>
+    <t>End reason</t>
+  </si>
+  <si>
+    <t>Statistic</t>
+  </si>
+  <si>
+    <t>To social housing</t>
+  </si>
+  <si>
+    <t>To private rented</t>
+  </si>
+  <si>
+    <t>To friends/family</t>
+  </si>
+  <si>
+    <t>Missing data/error</t>
+  </si>
+  <si>
+    <t>To external supported</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>To care/hospital</t>
+  </si>
+  <si>
+    <t>Abandoned</t>
+  </si>
+  <si>
+    <t>Evicted</t>
+  </si>
+  <si>
+    <t>Custody</t>
+  </si>
+  <si>
+    <t>Eligible (n)</t>
+  </si>
+  <si>
+    <t>Returned (n)</t>
   </si>
 </sst>
 </file>
@@ -404,18 +449,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -435,7 +480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -458,7 +503,7 @@
         <v>1617</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -481,7 +526,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -504,7 +549,7 @@
         <v>38.7</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -527,7 +572,790 @@
         <v>61.3</v>
       </c>
     </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>979</v>
+      </c>
+      <c r="D10">
+        <v>954</v>
+      </c>
+      <c r="E10">
+        <v>885</v>
+      </c>
+      <c r="F10">
+        <v>870</v>
+      </c>
+      <c r="G10">
+        <v>822</v>
+      </c>
+      <c r="H10">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>0.1</v>
+      </c>
+      <c r="D12">
+        <v>0.1</v>
+      </c>
+      <c r="E12">
+        <v>0.5</v>
+      </c>
+      <c r="F12">
+        <v>0.7</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>273</v>
+      </c>
+      <c r="D13">
+        <v>267</v>
+      </c>
+      <c r="E13">
+        <v>239</v>
+      </c>
+      <c r="F13">
+        <v>234</v>
+      </c>
+      <c r="G13">
+        <v>224</v>
+      </c>
+      <c r="H13">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>16</v>
+      </c>
+      <c r="H14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>0.4</v>
+      </c>
+      <c r="D15">
+        <v>1.9</v>
+      </c>
+      <c r="E15">
+        <v>3.8</v>
+      </c>
+      <c r="F15">
+        <v>4.3</v>
+      </c>
+      <c r="G15">
+        <v>7.1</v>
+      </c>
+      <c r="H15">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>364</v>
+      </c>
+      <c r="D16">
+        <v>358</v>
+      </c>
+      <c r="E16">
+        <v>345</v>
+      </c>
+      <c r="F16">
+        <v>339</v>
+      </c>
+      <c r="G16">
+        <v>322</v>
+      </c>
+      <c r="H16">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+      <c r="D17">
+        <v>26</v>
+      </c>
+      <c r="E17">
+        <v>59</v>
+      </c>
+      <c r="F17">
+        <v>68</v>
+      </c>
+      <c r="G17">
+        <v>77</v>
+      </c>
+      <c r="H17">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>3.3</v>
+      </c>
+      <c r="D18">
+        <v>7.3</v>
+      </c>
+      <c r="E18">
+        <v>17.1</v>
+      </c>
+      <c r="F18">
+        <v>20.1</v>
+      </c>
+      <c r="G18">
+        <v>23.9</v>
+      </c>
+      <c r="H18">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>74</v>
+      </c>
+      <c r="D19">
+        <v>74</v>
+      </c>
+      <c r="E19">
+        <v>70</v>
+      </c>
+      <c r="F19">
+        <v>68</v>
+      </c>
+      <c r="G19">
+        <v>62</v>
+      </c>
+      <c r="H19">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>17</v>
+      </c>
+      <c r="E20">
+        <v>17</v>
+      </c>
+      <c r="F20">
+        <v>17</v>
+      </c>
+      <c r="G20">
+        <v>15</v>
+      </c>
+      <c r="H20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>14.9</v>
+      </c>
+      <c r="D21">
+        <v>23</v>
+      </c>
+      <c r="E21">
+        <v>24.3</v>
+      </c>
+      <c r="F21">
+        <v>25</v>
+      </c>
+      <c r="G21">
+        <v>24.2</v>
+      </c>
+      <c r="H21">
+        <v>35.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>161</v>
+      </c>
+      <c r="D22">
+        <v>155</v>
+      </c>
+      <c r="E22">
+        <v>142</v>
+      </c>
+      <c r="F22">
+        <v>138</v>
+      </c>
+      <c r="G22">
+        <v>130</v>
+      </c>
+      <c r="H22">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>36</v>
+      </c>
+      <c r="F23">
+        <v>36</v>
+      </c>
+      <c r="G23">
+        <v>39</v>
+      </c>
+      <c r="H23">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <v>8.1</v>
+      </c>
+      <c r="D24">
+        <v>17.4</v>
+      </c>
+      <c r="E24">
+        <v>25.4</v>
+      </c>
+      <c r="F24">
+        <v>26.1</v>
+      </c>
+      <c r="G24">
+        <v>30</v>
+      </c>
+      <c r="H24">
+        <v>39.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>275</v>
+      </c>
+      <c r="D25">
+        <v>266</v>
+      </c>
+      <c r="E25">
+        <v>232</v>
+      </c>
+      <c r="F25">
+        <v>227</v>
+      </c>
+      <c r="G25">
+        <v>213</v>
+      </c>
+      <c r="H25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>34</v>
+      </c>
+      <c r="D26">
+        <v>48</v>
+      </c>
+      <c r="E26">
+        <v>61</v>
+      </c>
+      <c r="F26">
+        <v>61</v>
+      </c>
+      <c r="G26">
+        <v>71</v>
+      </c>
+      <c r="H26">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>12.4</v>
+      </c>
+      <c r="D27">
+        <v>18</v>
+      </c>
+      <c r="E27">
+        <v>26.3</v>
+      </c>
+      <c r="F27">
+        <v>26.9</v>
+      </c>
+      <c r="G27">
+        <v>33.3</v>
+      </c>
+      <c r="H27">
+        <v>43.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28">
+        <v>163</v>
+      </c>
+      <c r="D28">
+        <v>154</v>
+      </c>
+      <c r="E28">
+        <v>139</v>
+      </c>
+      <c r="F28">
+        <v>138</v>
+      </c>
+      <c r="G28">
+        <v>127</v>
+      </c>
+      <c r="H28">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>27</v>
+      </c>
+      <c r="D29">
+        <v>42</v>
+      </c>
+      <c r="E29">
+        <v>51</v>
+      </c>
+      <c r="F29">
+        <v>53</v>
+      </c>
+      <c r="G29">
+        <v>50</v>
+      </c>
+      <c r="H29">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30">
+        <v>16.6</v>
+      </c>
+      <c r="D30">
+        <v>27.3</v>
+      </c>
+      <c r="E30">
+        <v>36.7</v>
+      </c>
+      <c r="F30">
+        <v>38.4</v>
+      </c>
+      <c r="G30">
+        <v>39.4</v>
+      </c>
+      <c r="H30">
+        <v>47.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31">
+        <v>626</v>
+      </c>
+      <c r="D31">
+        <v>609</v>
+      </c>
+      <c r="E31">
+        <v>553</v>
+      </c>
+      <c r="F31">
+        <v>528</v>
+      </c>
+      <c r="G31">
+        <v>477</v>
+      </c>
+      <c r="H31">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32">
+        <v>59</v>
+      </c>
+      <c r="D32">
+        <v>126</v>
+      </c>
+      <c r="E32">
+        <v>218</v>
+      </c>
+      <c r="F32">
+        <v>230</v>
+      </c>
+      <c r="G32">
+        <v>223</v>
+      </c>
+      <c r="H32">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>9.4</v>
+      </c>
+      <c r="D33">
+        <v>20.7</v>
+      </c>
+      <c r="E33">
+        <v>39.4</v>
+      </c>
+      <c r="F33">
+        <v>43.6</v>
+      </c>
+      <c r="G33">
+        <v>46.8</v>
+      </c>
+      <c r="H33">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34">
+        <v>835</v>
+      </c>
+      <c r="D34">
+        <v>801</v>
+      </c>
+      <c r="E34">
+        <v>726</v>
+      </c>
+      <c r="F34">
+        <v>688</v>
+      </c>
+      <c r="G34">
+        <v>621</v>
+      </c>
+      <c r="H34">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35">
+        <v>164</v>
+      </c>
+      <c r="D35">
+        <v>246</v>
+      </c>
+      <c r="E35">
+        <v>328</v>
+      </c>
+      <c r="F35">
+        <v>334</v>
+      </c>
+      <c r="G35">
+        <v>323</v>
+      </c>
+      <c r="H35">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <v>19.6</v>
+      </c>
+      <c r="D36">
+        <v>30.7</v>
+      </c>
+      <c r="E36">
+        <v>45.2</v>
+      </c>
+      <c r="F36">
+        <v>48.5</v>
+      </c>
+      <c r="G36">
+        <v>52</v>
+      </c>
+      <c r="H36">
+        <v>65.40000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37">
+        <v>327</v>
+      </c>
+      <c r="D37">
+        <v>321</v>
+      </c>
+      <c r="E37">
+        <v>301</v>
+      </c>
+      <c r="F37">
+        <v>297</v>
+      </c>
+      <c r="G37">
+        <v>277</v>
+      </c>
+      <c r="H37">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38">
+        <v>32</v>
+      </c>
+      <c r="D38">
+        <v>69</v>
+      </c>
+      <c r="E38">
+        <v>131</v>
+      </c>
+      <c r="F38">
+        <v>146</v>
+      </c>
+      <c r="G38">
+        <v>148</v>
+      </c>
+      <c r="H38">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="D39">
+        <v>21.5</v>
+      </c>
+      <c r="E39">
+        <v>43.5</v>
+      </c>
+      <c r="F39">
+        <v>49.2</v>
+      </c>
+      <c r="G39">
+        <v>53.4</v>
+      </c>
+      <c r="H39">
+        <v>69.40000000000001</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A37:A39"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>